<commit_message>
additional columns on employee list
</commit_message>
<xml_diff>
--- a/public/template/employee/Employee List - Template.xlsx
+++ b/public/template/employee/Employee List - Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\MSS Compliance Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\vueportal\public\template\employee\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>employee_code</t>
   </si>
@@ -168,6 +168,24 @@
   </si>
   <si>
     <t>1987-08-29</t>
+  </si>
+  <si>
+    <t>educ_attain</t>
+  </si>
+  <si>
+    <t>school_attended</t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>bachelor's</t>
+  </si>
+  <si>
+    <t>ADMU</t>
+  </si>
+  <si>
+    <t>IT</t>
   </si>
 </sst>
 </file>
@@ -175,8 +193,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="172" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="174" formatCode="#,##0.00&quot; &quot;;&quot; (&quot;#,##0.00&quot;)&quot;;&quot; -&quot;#&quot; &quot;;@&quot; &quot;"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00&quot; &quot;;&quot; (&quot;#,##0.00&quot;)&quot;;&quot; -&quot;#&quot; &quot;;@&quot; &quot;"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -223,9 +241,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="174" fontId="2" fillId="0" borderId="0" applyFont="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -234,12 +252,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Comma" xfId="1"/>
@@ -521,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,9 +569,12 @@
     <col min="20" max="21" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -622,8 +647,17 @@
       <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="Y1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -695,6 +729,15 @@
       </c>
       <c r="X2" s="2" t="s">
         <v>45</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>